<commit_message>
[CSV] Research csv파일 미디어 부분 삭제
</commit_message>
<xml_diff>
--- a/Design/Tables/Research.xlsx
+++ b/Design/Tables/Research.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52CA286-23CC-4DA6-B6AD-AE917CDB0085}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47A4A6E-72C5-4107-A885-4B4631C04FB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,42 +75,6 @@
   </si>
   <si>
     <t>불안</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[미디어]장르</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인터뷰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여행</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>취미</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>음악</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드라마</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뉴스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>먹방</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 소개</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -608,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -646,55 +610,55 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="R1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="S1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="T1" t="s">
         <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -708,55 +672,55 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="N2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="O2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="S2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="T2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -1319,13 +1283,13 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10200</v>
+        <v>20100</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12">
-        <v>432</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1381,7 +1345,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>10201</v>
+        <v>20101</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -1396,16 +1360,16 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1443,7 +1407,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>10202</v>
+        <v>20102</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -1452,7 +1416,7 @@
         <v>432</v>
       </c>
       <c r="D14">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1461,22 +1425,22 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1505,7 +1469,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>10203</v>
+        <v>20103</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -1514,7 +1478,7 @@
         <v>432</v>
       </c>
       <c r="D15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1523,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1532,13 +1496,13 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1567,7 +1531,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>10204</v>
+        <v>20104</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -1576,7 +1540,7 @@
         <v>432</v>
       </c>
       <c r="D16">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1588,48 +1552,48 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>10205</v>
+        <v>20105</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -1644,57 +1608,57 @@
         <v>0</v>
       </c>
       <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0.5</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>7.5</v>
+      </c>
+      <c r="N17">
+        <v>0.8</v>
+      </c>
+      <c r="O17">
+        <v>-0.3</v>
+      </c>
+      <c r="P17">
+        <v>-0.75</v>
+      </c>
+      <c r="Q17">
+        <v>0.1</v>
+      </c>
+      <c r="R17">
         <v>0.2</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0.2</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0.2</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
       <c r="S17">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>10206</v>
+        <v>20106</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>432</v>
@@ -1706,60 +1670,60 @@
         <v>0</v>
       </c>
       <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0.5</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>5.5</v>
+      </c>
+      <c r="N18">
+        <v>0.7</v>
+      </c>
+      <c r="O18">
+        <v>-0.3</v>
+      </c>
+      <c r="P18">
+        <v>-0.75</v>
+      </c>
+      <c r="Q18">
+        <v>0.1</v>
+      </c>
+      <c r="R18">
         <v>0.2</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0.2</v>
-      </c>
-      <c r="I18">
-        <v>0.2</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
       <c r="S18">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>10207</v>
+        <v>30100</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>432</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1768,16 +1732,16 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1815,7 +1779,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>10208</v>
+        <v>30101</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -1824,25 +1788,25 @@
         <v>432</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="J20">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1877,28 +1841,28 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20100</v>
+        <v>30102</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>432</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1939,7 +1903,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>20101</v>
+        <v>30103</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
@@ -1957,10 +1921,10 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -2001,7 +1965,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>20102</v>
+        <v>30104</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
@@ -2019,22 +1983,22 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="K23">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -2063,7 +2027,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>20103</v>
+        <v>30105</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2087,16 +2051,16 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K24">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2125,7 +2089,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>20104</v>
+        <v>30106</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
@@ -2146,48 +2110,48 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="K25">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N25">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="O25">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="P25">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="Q25">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="R25">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S25">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="T25">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>20105</v>
+        <v>30107</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
@@ -2196,10 +2160,10 @@
         <v>432</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2211,51 +2175,51 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K26">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="O26">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="Q26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="R26">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="S26">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="T26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>20106</v>
+        <v>40100</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
       <c r="C27">
-        <v>432</v>
+        <v>0</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2279,45 +2243,45 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="N27">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="O27">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="P27">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="Q27">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="R27">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="S27">
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
       <c r="T27">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>30100</v>
+        <v>40101</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>432</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2335,10 +2299,10 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -2373,7 +2337,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>30101</v>
+        <v>40102</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
@@ -2382,13 +2346,13 @@
         <v>432</v>
       </c>
       <c r="D29">
-        <v>-0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2397,10 +2361,10 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>-0.05</v>
+        <v>0.1</v>
       </c>
       <c r="J29">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -2435,7 +2399,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>30102</v>
+        <v>40103</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
@@ -2444,25 +2408,25 @@
         <v>432</v>
       </c>
       <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>0.1</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
       <c r="F30">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="H30">
-        <v>0.35</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -2497,7 +2461,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30103</v>
+        <v>40104</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
@@ -2509,16 +2473,16 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G31">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>-0.15</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2559,7 +2523,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>30104</v>
+        <v>40105</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
@@ -2568,25 +2532,25 @@
         <v>432</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="G32">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -2621,7 +2585,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>30105</v>
+        <v>40106</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
@@ -2630,13 +2594,13 @@
         <v>432</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -2645,10 +2609,10 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>-0.05</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="J33">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -2683,7 +2647,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>30106</v>
+        <v>40107</v>
       </c>
       <c r="B34" t="s">
         <v>36</v>
@@ -2701,16 +2665,16 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="H34">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="I34">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -2745,7 +2709,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>30107</v>
+        <v>40108</v>
       </c>
       <c r="B35" t="s">
         <v>37</v>
@@ -2754,10 +2718,10 @@
         <v>432</v>
       </c>
       <c r="D35">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2769,10 +2733,10 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="J35">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -2807,22 +2771,22 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>40100</v>
+        <v>40109</v>
       </c>
       <c r="B36" t="s">
         <v>38</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>432</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2864,564 +2828,6 @@
         <v>0</v>
       </c>
       <c r="T36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>40101</v>
-      </c>
-      <c r="B37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37">
-        <v>432</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0.15</v>
-      </c>
-      <c r="J37">
-        <v>0.1</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
-      <c r="R37">
-        <v>0</v>
-      </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>40102</v>
-      </c>
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38">
-        <v>432</v>
-      </c>
-      <c r="D38">
-        <v>0.1</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>-0.2</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0.1</v>
-      </c>
-      <c r="J38">
-        <v>0.1</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="R38">
-        <v>0</v>
-      </c>
-      <c r="S38">
-        <v>0</v>
-      </c>
-      <c r="T38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>40103</v>
-      </c>
-      <c r="B39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39">
-        <v>432</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0.1</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0.1</v>
-      </c>
-      <c r="H39">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="I39">
-        <v>-0.25</v>
-      </c>
-      <c r="J39">
-        <v>0.1</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="R39">
-        <v>0</v>
-      </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>40104</v>
-      </c>
-      <c r="B40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40">
-        <v>432</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0.1</v>
-      </c>
-      <c r="F40">
-        <v>0.2</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>0</v>
-      </c>
-      <c r="S40">
-        <v>0</v>
-      </c>
-      <c r="T40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>40105</v>
-      </c>
-      <c r="B41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41">
-        <v>432</v>
-      </c>
-      <c r="D41">
-        <v>0.2</v>
-      </c>
-      <c r="E41">
-        <v>0.1</v>
-      </c>
-      <c r="F41">
-        <v>-0.2</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41">
-        <v>0</v>
-      </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="R41">
-        <v>0</v>
-      </c>
-      <c r="S41">
-        <v>0</v>
-      </c>
-      <c r="T41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>40106</v>
-      </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42">
-        <v>432</v>
-      </c>
-      <c r="D42">
-        <v>-0.15</v>
-      </c>
-      <c r="E42">
-        <v>0.1</v>
-      </c>
-      <c r="F42">
-        <v>0.1</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="J42">
-        <v>0.1</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42">
-        <v>0</v>
-      </c>
-      <c r="P42">
-        <v>0</v>
-      </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="R42">
-        <v>0</v>
-      </c>
-      <c r="S42">
-        <v>0</v>
-      </c>
-      <c r="T42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>40107</v>
-      </c>
-      <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43">
-        <v>432</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>-0.05</v>
-      </c>
-      <c r="H43">
-        <v>0.4</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-      <c r="P43">
-        <v>0</v>
-      </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
-      <c r="R43">
-        <v>0</v>
-      </c>
-      <c r="S43">
-        <v>0</v>
-      </c>
-      <c r="T43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>40108</v>
-      </c>
-      <c r="B44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44">
-        <v>432</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>-0.6</v>
-      </c>
-      <c r="J44">
-        <v>0.6</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
-      <c r="P44">
-        <v>0</v>
-      </c>
-      <c r="Q44">
-        <v>0</v>
-      </c>
-      <c r="R44">
-        <v>0</v>
-      </c>
-      <c r="S44">
-        <v>0</v>
-      </c>
-      <c r="T44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>40109</v>
-      </c>
-      <c r="B45" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45">
-        <v>432</v>
-      </c>
-      <c r="D45">
-        <v>-0.75</v>
-      </c>
-      <c r="E45">
-        <v>-0.3</v>
-      </c>
-      <c r="F45">
-        <v>0.75</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45">
-        <v>0</v>
-      </c>
-      <c r="N45">
-        <v>0</v>
-      </c>
-      <c r="O45">
-        <v>0</v>
-      </c>
-      <c r="P45">
-        <v>0</v>
-      </c>
-      <c r="Q45">
-        <v>0</v>
-      </c>
-      <c r="R45">
-        <v>0</v>
-      </c>
-      <c r="S45">
-        <v>0</v>
-      </c>
-      <c r="T45">
         <v>0</v>
       </c>
     </row>

</xml_diff>